<commit_message>
New results from gpt5
</commit_message>
<xml_diff>
--- a/reports/reconciliation_breaks_combined.xlsx
+++ b/reports/reconciliation_breaks_combined.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>priority</t>
   </si>
@@ -70,22 +70,19 @@
     <t>USD</t>
   </si>
   <si>
-    <t>Custody paid on 12,000 shares while NBIM booked 10,000, with the same dividend rate and tax, resulting in CHF 4,030 more cash at custody. Dates and rates match; the variance is driven by entitlement quantity.</t>
-  </si>
-  <si>
-    <t>Custody net cash is higher because custodian applied 20% tax while NBIM booked a total ~25% (22% WHT + ~2.985% local). This drives USD 5,181.50 (NBIM) vs USD 5,524.27 (custody).</t>
-  </si>
-  <si>
-    <t>PROPOSE_NBIM_CORRECTION</t>
+    <t>Custody paid dividend on 12,000 shares while entitlement should be 10,000; the CHF 4,030 net difference equals 2,000 shares × CHF 2.015 net/share.</t>
+  </si>
+  <si>
+    <t>Custody applied 20% tax (net QC 7,220,000 KRW) while NBIM applied ~25% total (22% WHT + ~2.985% local; net QC 6,769,950 KRW), leading to higher custody cash by 342.77 USD. Dates and lending flags do not explain the amount; this is a tax-rate application difference.</t>
   </si>
   <si>
     <t>DRAFT_CUSTODIAN_TICKET</t>
   </si>
   <si>
-    <t>NBIM likely under-booked entitlement by 2,000 shares. Please verify record-date holdings/transfers and update the entitlement or book a supplemental receipt for CHF 4,030. Note custody shows NOMINAL_BASIS 10,000 but amounts reflect 12,000; validate with UBS if needed.</t>
-  </si>
-  <si>
-    <t>Please confirm the actual tax rate and breakdown applied by HSBC Korea for KR7005930003 dividend ex 31.03.2025. Custody shows 20% withholding (net USD 5,524.27) while NBIM booked 22% WHT + ~2.985% local (~25% total), net USD 5,181.50. Advise if treaty/relief was applied or if local surtax is not applicable. If 20% is correct, we will adjust NBIM booking; if not, please correct custody records/cash and provide details. Cross-currency reversal flag noted; please confirm it does not affect the net tax outcome.</t>
+    <t>Please verify the dividend entitlement quantity at record date. Custody file states NOMINAL_BASIS 10,000 but amounts reflect 12,000 shares. If 2,000 shares were included in error, kindly advise reversal/adjustment; otherwise provide rationale (e.g., late trade or sub-account allocation). Event dates align on both sides (Ex 25-Apr-2025, Pay 29-Apr-2025).</t>
+  </si>
+  <si>
+    <t>Please ask custodian (CUST/HSBCKR) to confirm the correct Korean dividend withholding and local surtax for this event (Samsung Electronics, ex 31-Mar-2025, pay 20/25-May-2025). Their booking reflects 20% only, while NBIM expects ~25% total (22% WHT + local). Clarify whether local surtax and the additional 2% WHT component will be collected/adjusted, and whether any securities lending portion (2,000 shares) is treated differently. Cross-currency reversal noted but not the driver of the discrepancy.</t>
   </si>
 </sst>
 </file>
@@ -500,13 +497,13 @@
         <v>18</v>
       </c>
       <c r="H2">
-        <v>0.9</v>
+        <v>0.86</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
       </c>
       <c r="J2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -532,13 +529,13 @@
         <v>19</v>
       </c>
       <c r="H3">
-        <v>0.87</v>
+        <v>0.9</v>
       </c>
       <c r="I3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Clean up code + added to readme
</commit_message>
<xml_diff>
--- a/reports/reconciliation_breaks_combined.xlsx
+++ b/reports/reconciliation_breaks_combined.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t>priority</t>
   </si>
@@ -25,6 +25,12 @@
     <t>bank_account</t>
   </si>
   <si>
+    <t>custodian</t>
+  </si>
+  <si>
+    <t>organisation_name</t>
+  </si>
+  <si>
     <t>classification</t>
   </si>
   <si>
@@ -58,6 +64,18 @@
     <t>712345678</t>
   </si>
   <si>
+    <t>CUST/UBSCH</t>
+  </si>
+  <si>
+    <t>CUST/HSBCKR</t>
+  </si>
+  <si>
+    <t>Nestle SA</t>
+  </si>
+  <si>
+    <t>Samsung Electronics Co Ltd</t>
+  </si>
+  <si>
     <t>QUANTITY_OR_LENDING_MISMATCH</t>
   </si>
   <si>
@@ -70,19 +88,22 @@
     <t>USD</t>
   </si>
   <si>
-    <t>Custody paid dividend on 12,000 shares while entitlement should be 10,000; the CHF 4,030 net difference equals 2,000 shares × CHF 2.015 net/share.</t>
-  </si>
-  <si>
-    <t>Custody applied 20% tax (net QC 7,220,000 KRW) while NBIM applied ~25% total (22% WHT + ~2.985% local; net QC 6,769,950 KRW), leading to higher custody cash by 342.77 USD. Dates and lending flags do not explain the amount; this is a tax-rate application difference.</t>
+    <t>Custody cash reflects 12,000 shares (CHF 3.10 = CHF 37,200 gross; CHF 24,180 net) while NBIM booked 10,000 shares (CHF 31,000 gross; CHF 20,150 net). Dates, currency, and tax rate align; the mismatch is driven by entitlement quantity.</t>
+  </si>
+  <si>
+    <t>NBIM applied ~25% total tax (22% WHT + ~3% local) while custody applied 20%, resulting in higher cash at custody. The USD difference (~342.77) aligns with ~5% of gross in KRW.</t>
   </si>
   <si>
     <t>DRAFT_CUSTODIAN_TICKET</t>
   </si>
   <si>
-    <t>Please verify the dividend entitlement quantity at record date. Custody file states NOMINAL_BASIS 10,000 but amounts reflect 12,000 shares. If 2,000 shares were included in error, kindly advise reversal/adjustment; otherwise provide rationale (e.g., late trade or sub-account allocation). Event dates align on both sides (Ex 25-Apr-2025, Pay 29-Apr-2025).</t>
-  </si>
-  <si>
-    <t>Please ask custodian (CUST/HSBCKR) to confirm the correct Korean dividend withholding and local surtax for this event (Samsung Electronics, ex 31-Mar-2025, pay 20/25-May-2025). Their booking reflects 20% only, while NBIM expects ~25% total (22% WHT + local). Clarify whether local surtax and the additional 2% WHT component will be collected/adjusted, and whether any securities lending portion (2,000 shares) is treated differently. Cross-currency reversal noted but not the driver of the discrepancy.</t>
+    <t>PROPOSE_NBIM_CORRECTION</t>
+  </si>
+  <si>
+    <t>Please confirm the entitled quantity at record date and whether 2,000 shares were ineligible (e.g., on loan or acquired ex-date). Custody record shows LOAN_QUANTITY 0 and LENDING_PERCENTAGE 0 but cash calculated on 12,000, while NOMINAL_BASIS = 10,000. Request breakdown of entitlement vs. holding and correct the paid amount or issue an adjustment if 10,000 is correct. If 12,000 is confirmed as entitled, NBIM will adjust its booking accordingly. POSSIBLE_RESTITUTION flags appear unrelated to this quantity issue.</t>
+  </si>
+  <si>
+    <t>NBIM appears to have an extra local tax component (bringing total to ~25%). Please review KR dividend tax setup for this event and align to the rate applied by HSBC Korea (20%) or confirm the correct statutory/treaty rate. If 20% is confirmed, adjust NBIM booking and tax rates; if not, request custody to clarify their applied rate and any relief-at-source treatment.</t>
   </si>
 </sst>
 </file>
@@ -425,7 +446,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -433,16 +454,17 @@
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
-    <col min="7" max="7" width="80.7109375" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
-    <col min="9" max="9" width="26.7109375" customWidth="1"/>
-    <col min="10" max="10" width="48.7109375" customWidth="1"/>
+    <col min="4" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="80.7109375" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
+    <col min="11" max="11" width="26.7109375" customWidth="1"/>
+    <col min="12" max="12" width="48.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -473,69 +495,87 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:12">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2">
         <v>4030</v>
       </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2">
-        <v>0.86</v>
+      <c r="H2" t="s">
+        <v>22</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="J2">
+        <v>0.8</v>
+      </c>
+      <c r="K2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3">
         <v>342.77</v>
       </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3">
-        <v>0.9</v>
+      <c r="H3" t="s">
+        <v>23</v>
       </c>
       <c r="I3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="J3">
+        <v>0.76</v>
+      </c>
+      <c r="K3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>